<commit_message>
validacion rips cuenta 17
</commit_message>
<xml_diff>
--- a/2024 CONTRIBUTIVO ok.xlsx
+++ b/2024 CONTRIBUTIVO ok.xlsx
@@ -1,24 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AIC-PUTUMAYO\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\bogota\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24711221-B67C-47A3-B2FD-7427807679F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7872E4-34FF-4F04-B117-AC5B75BC6269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FE22F8EB-AFB2-4531-B872-74E578C2F16A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{FE22F8EB-AFB2-4531-B872-74E578C2F16A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -878,13 +888,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{361F6DE0-F27C-4022-BEBB-1D8D58549D20}">
   <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C15:C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -988,7 +998,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>166</v>
       </c>
@@ -1082,7 +1092,7 @@
         <v>1120101438</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>167</v>
       </c>
@@ -1176,7 +1186,7 @@
         <v>1120101438</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>1295</v>
       </c>
@@ -1270,7 +1280,7 @@
         <v>18103338</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>1296</v>
       </c>
@@ -1364,7 +1374,7 @@
         <v>18103338</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>1428</v>
       </c>
@@ -1458,7 +1468,7 @@
         <v>1125412066</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>1959</v>
       </c>
@@ -1552,7 +1562,7 @@
         <v>1124856439</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>1960</v>
       </c>
@@ -1646,7 +1656,7 @@
         <v>1124856439</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>2067</v>
       </c>
@@ -1738,7 +1748,7 @@
         <v>18112358</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>2068</v>
       </c>
@@ -1854,4 +1864,44 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569656A0-7B66-4A04-A469-558D2EF052A1}">
+  <dimension ref="A2:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>1120101438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18">
+        <v>18103338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18">
+        <v>1125412066</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18">
+        <v>1124856439</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
+        <v>18112358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>